<commit_message>
positive and negative login
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/TC01.xlsx
+++ b/src/main/resources/dataSheets/TC01.xlsx
@@ -1,41 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lokthy/Documents/Personal/Automation Frameworks/AppiumDec2020/src/main/resources/dataSheets/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0D46CE-3411-1440-9291-018E8222BADB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0E8BD349-DE39-48BE-9801-F1A722EE8DFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{2B02C3BB-63FE-7140-94EE-4236C8474EDA}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="20790" windowHeight="11820" xr2:uid="{2B02C3BB-63FE-7140-94EE-4236C8474EDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>UserName</t>
   </si>
@@ -43,16 +29,13 @@
     <t>Password</t>
   </si>
   <si>
-    <t>rajkumar@testleaf.com</t>
+    <t>Admin@123</t>
   </si>
   <si>
-    <t>Leaf@123</t>
+    <t>fsqa1tpn@gmail.com</t>
   </si>
   <si>
-    <t>lokesh@testleaf.com</t>
-  </si>
-  <si>
-    <t>Hello@123</t>
+    <t>fsssacct3@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -418,15 +401,15 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,20 +417,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
how to play added
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/TC01.xlsx
+++ b/src/main/resources/dataSheets/TC01.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0E8BD349-DE39-48BE-9801-F1A722EE8DFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CE530BD8-E806-4DC5-9D43-FEF61D2FBDEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="20790" windowHeight="11820" xr2:uid="{2B02C3BB-63FE-7140-94EE-4236C8474EDA}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="20790" windowHeight="11820" xr2:uid="{2B02C3BB-63FE-7140-94EE-4236C8474EDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
google sign in added
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/TC01.xlsx
+++ b/src/main/resources/dataSheets/TC01.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CE530BD8-E806-4DC5-9D43-FEF61D2FBDEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssivaramakrishnan\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8BDC9C-BE70-4E42-956B-5091EFE89160}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="20790" windowHeight="11820" xr2:uid="{2B02C3BB-63FE-7140-94EE-4236C8474EDA}"/>
+    <workbookView xWindow="5115" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{2B02C3BB-63FE-7140-94EE-4236C8474EDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>UserName</t>
   </si>
@@ -33,9 +37,6 @@
   </si>
   <si>
     <t>fsqa1tpn@gmail.com</t>
-  </si>
-  <si>
-    <t>fsssacct3@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -401,7 +402,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -419,26 +420,20 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{4DE231DB-3E77-F94C-B627-801BFE92BFBA}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{6C3DCD2A-E3FC-A944-B0A1-156BED3F4CFE}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{808D9039-7A70-6946-B13B-66397101A843}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{4E721FC6-C664-6347-AB41-2679A15E3629}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>